<commit_message>
14 translate  XY | 17 direction _ degrees
</commit_message>
<xml_diff>
--- a/RevitDynamo/14files/relative_values.xlsx
+++ b/RevitDynamo/14files/relative_values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmsil\Desktop\bsp3\RevitDynamo\14files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67118EC-54C4-4835-A0F4-853A589F8188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66562699-5D83-4CE0-83AD-70EA736A194B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16635" yWindow="9795" windowWidth="19605" windowHeight="15345" xr2:uid="{A7A23B64-5B2A-4164-A763-E7FBE671D2B7}"/>
+    <workbookView xWindow="16650" yWindow="5370" windowWidth="19605" windowHeight="15345" xr2:uid="{A7A23B64-5B2A-4164-A763-E7FBE671D2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Wall" sheetId="6" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,10 +623,10 @@
         <v>58</v>
       </c>
       <c r="P2">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>-200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>